<commit_message>
Banco de dados alterado
</commit_message>
<xml_diff>
--- a/Documentação/Backlog.xlsx
+++ b/Documentação/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22021"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Documents\GIT\BlindMarket\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_51364A4E430207B3184EB461F19E65EA0B59046C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79518C16-CE21-4816-BB3E-90C2D220259B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14252B2-0FAE-433F-A6B7-8C1A64AE65AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,9 +222,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +512,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="106.140625" bestFit="1" customWidth="1"/>
@@ -519,7 +520,7 @@
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,7 +536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -543,7 +544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -551,7 +552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -559,15 +560,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -575,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -583,7 +584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -591,12 +592,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -607,7 +608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -618,7 +619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -629,7 +630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -640,7 +641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -651,7 +652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -662,12 +663,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -678,7 +679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -689,7 +690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -700,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -711,7 +712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -722,7 +723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -733,7 +734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -744,7 +745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -755,7 +756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -766,7 +767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -777,7 +778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
@@ -788,7 +789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>11</v>
       </c>
@@ -799,7 +800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12</v>
       </c>
@@ -810,12 +811,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -826,7 +827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -837,7 +838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -848,7 +849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -859,7 +860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -870,12 +871,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -886,7 +887,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -897,7 +898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -908,7 +909,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -919,7 +920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -932,5 +933,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>